<commit_message>
(Operaciones Relativas a los Afiliados) - se implementa metodo listar ascendente el cual recorre el arbol - se implementa test del metodo - se agrega duda de formato de impresion de listado
</commit_message>
<xml_diff>
--- a/Obligatorio Algoritmos 2/Dudas.xlsx
+++ b/Obligatorio Algoritmos 2/Dudas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Facundo\Desktop\Obligatorio Algoritmos\Obligatorio Algoritmos 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Facundo\Desktop\Obligatorio-Algoritmos-2\Obligatorio Algoritmos 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Solucionada</t>
   </si>
@@ -52,6 +52,11 @@
     <t>La lentra dice de forma explicita que no se debera loguear nada, sin embargo el metodo 
 BUSCAR AFILIADO pide que se devuelvan la cantidad de movimiento 
 realizados para encontrar al afiliado asi como tambien sus datos, es incorrecto loguear ducha informacion en la consola ?</t>
+  </si>
+  <si>
+    <t>Se puede cambiar el formato del listado para que tenga un espacio antes y despues
+del " | " y tmb tuvimos que inicializar el valorString ya que sino imprimia null al
+inicio del listado</t>
   </si>
 </sst>
 </file>
@@ -412,7 +417,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,10 +523,14 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+    <row r="8" spans="1:8" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="4"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>

</xml_diff>

<commit_message>
(Operaciones Red) - se implementa en sistema agregar canalera y sus test - se actualiza excel dudas
</commit_message>
<xml_diff>
--- a/Obligatorio Algoritmos 2/Dudas.xlsx
+++ b/Obligatorio Algoritmos 2/Dudas.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Facundo\Desktop\Obligatorio-Algoritmos-2\Obligatorio Algoritmos 2\"/>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Solucionada</t>
   </si>
@@ -57,12 +57,27 @@
     <t>Se puede cambiar el formato del listado para que tenga un espacio antes y despues
 del " | " y tmb tuvimos que inicializar el valorString ya que sino imprimia null al
 inicio del listado</t>
+  </si>
+  <si>
+    <t>Es necesario aclarar PRE y POS condiciones de cada metodo de la clase sistema</t>
+  </si>
+  <si>
+    <t>Documentacion en PDF?, ante se pedia con eleccion de estructuras y fundamentos, letra no pide.</t>
+  </si>
+  <si>
+    <t>Calclar max puntos del grafo, for o contador ??</t>
+  </si>
+  <si>
+    <t>E.equals()nde vertice?? Es por corrdX/coordY ????</t>
+  </si>
+  <si>
+    <t>NodoCritico ?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -417,17 +432,17 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="105.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" customWidth="1"/>
+    <col min="2" max="2" width="105.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -437,7 +452,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -453,7 +468,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -467,7 +482,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -481,7 +496,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -495,7 +510,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -509,7 +524,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -523,7 +538,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="54.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -537,57 +552,77 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+    <row r="9" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="4"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+    <row r="10" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="4"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+    <row r="11" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="4"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+    <row r="12" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="4"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+    <row r="13" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="4"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -597,7 +632,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -607,7 +642,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -617,7 +652,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -627,7 +662,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -637,7 +672,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -647,7 +682,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -657,7 +692,7 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -667,7 +702,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -677,7 +712,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -689,6 +724,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
(Operaciones Red) - Se implementa registrarTramo en sistema (no terminado) - se implementan tests (no terminado)
</commit_message>
<xml_diff>
--- a/Obligatorio Algoritmos 2/Dudas.xlsx
+++ b/Obligatorio Algoritmos 2/Dudas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Solucionada</t>
   </si>
@@ -72,6 +72,27 @@
   </si>
   <si>
     <t>NodoCritico ?</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Suficiente</t>
+  </si>
+  <si>
+    <t>Regex [.]</t>
+  </si>
+  <si>
+    <t>No es Necesario</t>
+  </si>
+  <si>
+    <t>Ya esta</t>
+  </si>
+  <si>
+    <t>Feo</t>
   </si>
 </sst>
 </file>
@@ -438,8 +459,8 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.88671875" customWidth="1"/>
-    <col min="2" max="2" width="105.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="106.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -475,7 +496,9 @@
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -489,7 +512,9 @@
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -503,7 +528,9 @@
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -517,7 +544,9 @@
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -531,7 +560,9 @@
       <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -545,21 +576,25 @@
       <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -573,7 +608,9 @@
       <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -587,7 +624,9 @@
       <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -601,7 +640,9 @@
       <c r="B12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>

</xml_diff>